<commit_message>
Include rows with object ID in the imported rows
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/permissions-valid.xlsx
+++ b/packages/sync-server/__tests__/importers/permissions-valid.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -83,6 +83,27 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>new-patients</t>
+  </si>
+  <si>
+    <t>SurveyResponse</t>
+  </si>
+  <si>
+    <t>ncd-screening</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Survey</t>
   </si>
   <si>
     <t>SucceedEvenThoughCapitalY</t>
@@ -110,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -129,7 +150,23 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -148,14 +185,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
@@ -382,9 +435,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="33.25"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1443,9 +1494,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.63"/>
     <col customWidth="1" min="2" max="2" width="24.75"/>
-    <col customWidth="1" min="3" max="3" width="12.63"/>
     <col customWidth="1" min="4" max="4" width="68.0"/>
-    <col customWidth="1" min="5" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1470,7 +1519,7 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1481,7 +1530,7 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1518,6 +1567,8 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1529,6 +1580,8 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1574,6 +1627,8 @@
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1585,6 +1640,8 @@
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1613,6 +1670,7 @@
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1627,6 +1685,7 @@
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1651,51 +1710,154 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
+      <c r="B22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>

</xml_diff>